<commit_message>
Feature/training service advanced (#39)
* after fix

* after some config

* finishing feature

* Final touches

* last but not least touches
</commit_message>
<xml_diff>
--- a/training-service/src/main/resources/Data.xlsx
+++ b/training-service/src/main/resources/Data.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26130"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Nour\Documents\Project\1.2\Biochar-backend\training-service\documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Nour\Documents\Project\1.3\Biochar-backend\training-service\src\main\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{75385299-6E2A-48CF-ACDB-E171741B2058}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C11AF5A-22D2-4E6C-9CC5-19135684F8EA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1560" yWindow="1560" windowWidth="15375" windowHeight="7875" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="22">
   <si>
     <t>Title</t>
   </si>
@@ -34,9 +34,6 @@
   </si>
   <si>
     <t>Complexity</t>
-  </si>
-  <si>
-    <t>Priority</t>
   </si>
   <si>
     <t>Anesthesiology</t>
@@ -422,8 +419,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D20"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
-      <selection activeCell="A15" sqref="A15"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -444,103 +441,110 @@
       <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
-        <v>3</v>
-      </c>
+      <c r="D1" s="1"/>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>22</v>
+        <v>21</v>
+      </c>
+      <c r="C2">
+        <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C3">
         <v>4</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>5</v>
+        <v>4</v>
+      </c>
+      <c r="C4">
+        <v>6</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="20" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
   </sheetData>

</xml_diff>